<commit_message>
Added a slection of problem instances, compared parameters
</commit_message>
<xml_diff>
--- a/prob-instances.xlsx
+++ b/prob-instances.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goson\Desktop\git\param-struct-cvxminlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9704E611-882B-4538-B6BC-51531DE16BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00511C8D-074F-4F9D-A3A9-81216BB857CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B275DA15-9E9C-498A-91BF-3EB439796FC2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B275DA15-9E9C-498A-91BF-3EB439796FC2}"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="1" r:id="rId1"/>
     <sheet name="Filtered (Table)" sheetId="2" r:id="rId2"/>
     <sheet name="Stats from t1" sheetId="5" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Stats from t1'!$D$3:$D$287</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Stats from t1'!$F$3:$F$287</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1230,7 +1234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1240,16 +1244,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1264,8 +1271,2687 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Stats from t1'!$D$3:$D$287</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="285"/>
+                <c:pt idx="0">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>67.56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16.03</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90.26</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>90.33</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>21.84</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18.45</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.58</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10.66</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>90.21</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>89.99</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>90.14</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>90.18</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90.16</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>74.72</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>34.270000000000003</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>34.31</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>90.16</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>90.02</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>90.02</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>90.16</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>90.24</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>90.15</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>90.15</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>11.14</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>86.97</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>90.01</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>90.02</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>5.57</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>5.29</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>11.32</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>7.82</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>14.65</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>90.18</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>90.15</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>16.23</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>76.760000000000005</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>90.11</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>41.57</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>90.16</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>90.17</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>90.23</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>90.04</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>90.11</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>90.15</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>90.18</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>90.14</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>90.12</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>90.05</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>90.26</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>90.31</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>90.13</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>11.16</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>72.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>90.54</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>3.32</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>7.82</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2.21</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>38.14</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>13.67</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>35.020000000000003</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>35.090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>7.89</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1.64</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>90.18</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>32.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>90.1</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>69.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>65.53</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>21.91</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>90.07</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>53.34</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>90.08</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>90.03</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>90.19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Stats from t1'!$F$3:$F$287</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="285"/>
+                <c:pt idx="0">
+                  <c:v>0.113999843597412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.078999996185303</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.093999862670898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.082000017166095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.0879998207092</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.082000017166095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.232000112533498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.845999956130896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.285000085830603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19099998474120999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59099984169006303</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.8000049591064398E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90.266000032424898</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.695000171661306</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>91.013999938964801</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>91.295000076293903</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6419999599456701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2750000953674301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.1949999332427</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9399998188018699</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.325000047683702</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.088999986648503</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5870001316070499</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.9660000801086399</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90.286000013351398</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41.600999832153299</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>90.383000135421696</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>90.085999965667696</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.177999973297119</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.261000156402587</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.22000002861022899</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>90.309999942779498</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.296999931335449</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.35400009155273399</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.271000146865844</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39.861000061035099</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.404000043869018</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>90.102999925613403</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.337000131607055</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.8409998416900599</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.27600002288818298</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.90700006484985296</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.24500012397766099</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.0999870300292899E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.23300004005432101</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>90.119999885558997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>90.101999998092595</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.45000004768371</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.6430001258850098</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.14299988746643</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.7000131607055595E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.14199995994567799</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53299999237060502</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>94.888999938964801</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.36199998855590798</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.202000141143798</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.25900006294250399</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.4809999465942301</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.575999975204467</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15.046999931335399</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>90.164999961852999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>90.095999956130896</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>90.194999933242798</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>90.177999973297105</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>90.166999816894503</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>90.143999814987097</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>90.180999994277897</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>90.148000001907306</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>90.1520001888275</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>90.167000055313096</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>90.135999917983995</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>90.189000129699707</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>90.150000095367403</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>90.145999908447195</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>90.144000053405705</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>90.153000116348196</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>90.197999954223604</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>90.200999975204397</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>90.226000070571899</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>90.180000066757202</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>90.152999877929602</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>90.230999946594196</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>90.221999883651705</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>90.958999872207599</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.26399993896484297</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.13100004196166901</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>15.0739998817443</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>90.138000011444007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90.098000049590993</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90.096999883651705</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>90.138000011444007</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>90.131000041961599</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>90.145999908447195</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.11899995803832999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>90.335000038146902</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>90.898999929428101</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>90.132999897003103</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>90.125</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>90.189999818801795</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>90.185000181198106</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>90.164999961852999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>90.194000005722003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>90.189000129699707</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8.5999965667724595E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.187000036239624</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.460999965667724</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.51099991798400801</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.27200007438659601</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>90.184999942779498</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>90.180999994277897</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>90.173000097274695</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>90.144999980926499</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>90.1789999008178</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>90.177000045776296</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>90.177000045776296</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>90.197000026702796</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>90.219000101089406</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>90.115000009536701</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>90.225999832153306</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.95499992370605402</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.24399995803832999</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3.268000125885</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2.63000011444091</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>90.235000133514404</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2.4019999504089302</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>90.332000017166095</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.3859999179839999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>90.460000038146902</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.296999931335449</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3.2089998722076398</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1.95100021362304</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>90.258000135421696</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4.7070000171661297</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>90.226999998092595</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.48600006103515</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>90.5099999904632</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.53500008583068803</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6.3740000724792401</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.0059998035430899</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>90.269999980926499</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>8.4980001449584908</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>90.395000219344993</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>5.2929999828338596</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>90.582999944686804</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1.2890000343322701</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>11.132999897003099</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.6319999694824201</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>90.319000005722003</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>11.853000164031901</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>90.427999973297105</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>8.1369998455047607</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>90.654999971389699</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.40100002288818</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>16.414000034332201</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.2409999370574898</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>90.410000085830603</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>90.522000074386597</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>90.730999946594196</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.59699988365173295</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>18.942999839782701</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2.83500003814697</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>90.388999938964801</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>7.8619999885559002</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>90.592999935150104</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>16.2209999561309</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>90.9189999103546</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.6029999256134</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.47900009155273399</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>8.7269999980926496</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.0420000553131099</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>90.178000211715698</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>5.5009999275207502</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>90.230999946594196</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>81.906999826431203</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>90.316999912261906</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>90.144000053405705</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>90.407999992370605</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>90.153000116348196</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>90.494999885558997</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>90.177999973297105</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>90.097000122070298</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>90.088000059127793</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>90.088999986648503</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>90.338999986648503</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>90.101000070571899</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>90.623999834060598</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>90.088999986648503</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>90.0910000801086</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>90.111999988555894</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>90.116000175476003</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>90.165999889373694</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>90.217999935150104</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>90.657999992370605</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>90.307999849319401</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>90.617999792098999</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>90.286000013351398</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>90.366999864578204</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>91.381999969482393</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>90.214999914169297</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>90.1689999103546</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>90.336999893188406</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>90.927999973297105</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>93.521000146865802</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>91.031000137329102</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>7.9319999217986998</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>90.211999893188406</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>90.171000003814697</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>90.233000040054307</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>90.221000194549504</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>90.243999958038302</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>90.194999933242798</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>90.184000015258704</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>90.199999809265094</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>90.309999942779498</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.14399981498718201</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.14100003242492601</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.12699985504150299</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>9.5999956130981404E-2</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>8.8999986648559501E-2</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>8.0000162124633706E-2</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.18499994277954099</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.105000019073486</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.72000002861022905</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9.9999904632568304E-2</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>33.3580000400543</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>90.826000213623004</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.12700009346008301</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>90.161999940872093</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.11599993705749501</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.115000009536743</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.11199998855590799</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.120999813079833</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.123999834060668</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.13599991798400801</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.138999938964843</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.230999946594238</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.118000030517578</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.123000144958496</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.14499998092651301</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.224999904632568</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.17499995231628401</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.414000034332275</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.212000131607055</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.60299992561340299</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.12999987602233801</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.14199995994567799</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.200999975204467</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.29999995231628401</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.27300000190734802</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.42499995231628401</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.384999990463256</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.80900001525878895</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.183000087738037</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.17000007629394501</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.33299994468688898</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.49099993705749501</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.38199996948242099</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.76300001144409102</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.46500015258789001</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>2.21900010108947</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.27999997138977001</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0.230999946594238</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.50600004196166903</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>2.0469999313354399</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.94299983978271396</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1.63499999046325</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1.7609999179839999</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>10.050000190734799</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.47399997711181602</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.51999998092651301</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1.0829999446868801</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>2.8279998302459699</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>4.1059999465942303</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>90.241000175476003</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>5.5290000438690097</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>90.4389998912811</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.13100004196166901</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.12599992752075101</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.20899987220764099</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3.4169998168945299</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.193000078201293</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>0.67599987983703602</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.19400000572204501</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>19.121000051498399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-040D-4646-8150-C40F2AFBBCF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1864948160"/>
+        <c:axId val="1864953440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1864948160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>BARON</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> SOLVE TIME</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1864953440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1864953440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>OUTER APPROXIMATION SOLVE TIME</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1864948160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69466CC2-343A-E889-7D7A-9891C5DE1261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D13CA597-DA8D-417F-A8F5-2ADD463832B8}" name="Table1" displayName="Table1" ref="B2:G368" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D13CA597-DA8D-417F-A8F5-2ADD463832B8}" name="Table1" displayName="Table1" ref="B2:G368" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="B2:G368" xr:uid="{D13CA597-DA8D-417F-A8F5-2ADD463832B8}">
     <filterColumn colId="4">
       <filters>
@@ -1542,7 +4228,7 @@
     <tableColumn id="1" xr3:uid="{F4F40257-F589-4190-90C5-4FC4D0C4D0E6}" name="Instance Name"/>
     <tableColumn id="2" xr3:uid="{60382085-0BE9-42E8-9EA0-EA048A008700}" name="Instance Number"/>
     <tableColumn id="3" xr3:uid="{26BB00D0-C325-40BB-AFF8-1DE19A4EAB68}" name="Solve Time"/>
-    <tableColumn id="4" xr3:uid="{556B40FC-634E-436C-9C40-9962AF37F006}" name="Objective" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{556B40FC-634E-436C-9C40-9962AF37F006}" name="Objective" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{313EB44C-C18E-43B3-B883-95729C568D53}" name="Solve Time2"/>
     <tableColumn id="6" xr3:uid="{9D0C3362-996D-4DDB-BC77-D2059B4FA743}" name="Objective3"/>
   </tableColumns>
@@ -16644,8 +19330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F82FCC4-5187-43DA-A162-AB6B198D8548}">
   <dimension ref="B1:P287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="J261" sqref="J261"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16813,10 +19499,10 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="5" t="s">
         <v>339</v>
       </c>
     </row>
@@ -16855,11 +19541,11 @@
         <f t="shared" si="3"/>
         <v>BR</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="5">
         <f>COUNTIF(K:K, "BR")</f>
         <v>65</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="5">
         <f>COUNTIF(K:K, "OA")</f>
         <v>104</v>
       </c>
@@ -26990,5 +29676,7 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>